<commit_message>
ddl script of building template and post property
</commit_message>
<xml_diff>
--- a/rsa-realty-release/2020/01/doc/Lookup_v3.xlsx
+++ b/rsa-realty-release/2020/01/doc/Lookup_v3.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="263">
   <si>
     <t>DATA_TYPE</t>
   </si>
@@ -3309,6 +3309,54 @@
       </rPr>
       <t>');</t>
     </r>
+  </si>
+  <si>
+    <t>YES_NO_NO_DATA_TYPE</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('YES_NO_NO_DATA_TYPE', '-1', 'No Data', 'DEFAULT', '', 'COMMON', 'COMMON', '1', 'Active', 'System-User', 'System-User');</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('YES_NO_NO_DATA_TYPE', '1', 'Yes', 'DEFAULT', '', 'COMMON', 'COMMON', '1', 'Active', 'System-User', 'System-User');</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('YES_NO_NO_DATA_TYPE', '2', 'No', 'DEFAULT', '', 'COMMON', 'COMMON', '1', 'Active', 'System-User', 'System-User');</t>
+  </si>
+  <si>
+    <t>PROPERTY_MAINTENANCE_PERIOD_TYPE</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('PROPERTY_MAINTENANCE_PERIOD_TYPE', '-1', 'No Data', 'DEFAULT', '', 'REALTY', 'PROPERTY', '1', 'Active', 'System-User', 'System-User');</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('PROPERTY_MAINTENANCE_PERIOD_TYPE', '1', 'Monthly', 'DEFAULT', '', 'REALTY', 'PROPERTY', '1', 'Active', 'System-User', 'System-User');</t>
+  </si>
+  <si>
+    <t>Quartly</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('PROPERTY_MAINTENANCE_PERIOD_TYPE', '2', 'Quartly', 'DEFAULT', '', 'REALTY', 'PROPERTY', '1', 'Active', 'System-User', 'System-User');</t>
+  </si>
+  <si>
+    <t>Yearly</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('PROPERTY_MAINTENANCE_PERIOD_TYPE', '3', 'Yearly', 'DEFAULT', '', 'REALTY', 'PROPERTY', '1', 'Active', 'System-User', 'System-User');</t>
+  </si>
+  <si>
+    <t>POST_PROPERTY_STATUS</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('POST_PROPERTY_STATUS', '-1', 'No Data', 'DEFAULT', '', 'REALTY', 'PROPERTY', '1', 'Active', 'System-User', 'System-User');</t>
+  </si>
+  <si>
+    <t>INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) VALUES ('POST_PROPERTY_STATUS', '', '', '', '', 'REALTY', 'PROPERTY', '1', 'Active', 'System-User', 'System-User');</t>
   </si>
   <si>
     <t>SEQ_ID</t>
@@ -4845,13 +4893,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N108"/>
+  <dimension ref="A1:N114"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.3281" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5391" style="1" customWidth="1"/>
     <col min="3" max="3" width="31.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="1" customWidth="1"/>
@@ -8965,53 +9013,350 @@
         <v>236</v>
       </c>
     </row>
-    <row r="106" ht="14.7" customHeight="1">
-      <c r="A106" s="8"/>
-      <c r="B106" s="8"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
+    <row r="106" ht="38.7" customHeight="1">
+      <c r="A106" t="s" s="3">
+        <v>237</v>
+      </c>
+      <c r="B106" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C106" t="s" s="3">
+        <v>53</v>
+      </c>
+      <c r="D106" t="s" s="3">
+        <v>17</v>
+      </c>
       <c r="E106" s="8"/>
-      <c r="F106" s="8"/>
-      <c r="G106" s="8"/>
-      <c r="H106" s="8"/>
-      <c r="I106" s="8"/>
-      <c r="J106" s="8"/>
+      <c r="F106" t="s" s="3">
+        <v>106</v>
+      </c>
+      <c r="G106" t="s" s="3">
+        <v>106</v>
+      </c>
+      <c r="H106" s="9">
+        <v>1</v>
+      </c>
+      <c r="I106" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J106" t="s" s="3">
+        <v>21</v>
+      </c>
       <c r="K106" s="8"/>
-      <c r="L106" s="8"/>
+      <c r="L106" t="s" s="3">
+        <v>21</v>
+      </c>
       <c r="M106" s="8"/>
-      <c r="N106" s="8"/>
-    </row>
-    <row r="107" ht="14.7" customHeight="1">
-      <c r="A107" s="8"/>
-      <c r="B107" s="8"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
+      <c r="N106" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A106,"', '",B106,"', '",C106,"', '",D106,"', '",E106,"', '",F106,"', '",G106,"', '",H106,"', '",I106,"', '",J106,"', '",L106,"');")</f>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="107" ht="38.7" customHeight="1">
+      <c r="A107" t="s" s="3">
+        <v>237</v>
+      </c>
+      <c r="B107" s="9">
+        <v>1</v>
+      </c>
+      <c r="C107" t="s" s="3">
+        <v>239</v>
+      </c>
+      <c r="D107" t="s" s="3">
+        <v>17</v>
+      </c>
       <c r="E107" s="8"/>
-      <c r="F107" s="8"/>
-      <c r="G107" s="8"/>
-      <c r="H107" s="8"/>
-      <c r="I107" s="8"/>
-      <c r="J107" s="8"/>
+      <c r="F107" t="s" s="3">
+        <v>106</v>
+      </c>
+      <c r="G107" t="s" s="3">
+        <v>106</v>
+      </c>
+      <c r="H107" s="9">
+        <v>1</v>
+      </c>
+      <c r="I107" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J107" t="s" s="3">
+        <v>21</v>
+      </c>
       <c r="K107" s="8"/>
-      <c r="L107" s="8"/>
+      <c r="L107" t="s" s="3">
+        <v>21</v>
+      </c>
       <c r="M107" s="8"/>
-      <c r="N107" s="8"/>
-    </row>
-    <row r="108" ht="14.7" customHeight="1">
-      <c r="A108" s="8"/>
-      <c r="B108" s="8"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="8"/>
+      <c r="N107" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A107,"', '",B107,"', '",C107,"', '",D107,"', '",E107,"', '",F107,"', '",G107,"', '",H107,"', '",I107,"', '",J107,"', '",L107,"');")</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="108" ht="38.7" customHeight="1">
+      <c r="A108" t="s" s="3">
+        <v>237</v>
+      </c>
+      <c r="B108" s="9">
+        <v>2</v>
+      </c>
+      <c r="C108" t="s" s="3">
+        <v>161</v>
+      </c>
+      <c r="D108" t="s" s="3">
+        <v>17</v>
+      </c>
       <c r="E108" s="8"/>
-      <c r="F108" s="8"/>
-      <c r="G108" s="8"/>
-      <c r="H108" s="8"/>
-      <c r="I108" s="8"/>
-      <c r="J108" s="8"/>
+      <c r="F108" t="s" s="3">
+        <v>106</v>
+      </c>
+      <c r="G108" t="s" s="3">
+        <v>106</v>
+      </c>
+      <c r="H108" s="9">
+        <v>1</v>
+      </c>
+      <c r="I108" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J108" t="s" s="3">
+        <v>21</v>
+      </c>
       <c r="K108" s="8"/>
-      <c r="L108" s="8"/>
+      <c r="L108" t="s" s="3">
+        <v>21</v>
+      </c>
       <c r="M108" s="8"/>
-      <c r="N108" s="8"/>
+      <c r="N108" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A108,"', '",B108,"', '",C108,"', '",D108,"', '",E108,"', '",F108,"', '",G108,"', '",H108,"', '",I108,"', '",J108,"', '",L108,"');")</f>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="109" ht="38.7" customHeight="1">
+      <c r="A109" t="s" s="3">
+        <v>242</v>
+      </c>
+      <c r="B109" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C109" t="s" s="3">
+        <v>53</v>
+      </c>
+      <c r="D109" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="E109" s="8"/>
+      <c r="F109" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G109" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="H109" s="9">
+        <v>1</v>
+      </c>
+      <c r="I109" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J109" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="K109" s="8"/>
+      <c r="L109" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="M109" s="8"/>
+      <c r="N109" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A109,"', '",B109,"', '",C109,"', '",D109,"', '",E109,"', '",F109,"', '",G109,"', '",H109,"', '",I109,"', '",J109,"', '",L109,"');")</f>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="110" ht="38.7" customHeight="1">
+      <c r="A110" t="s" s="3">
+        <v>242</v>
+      </c>
+      <c r="B110" s="9">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s" s="3">
+        <v>244</v>
+      </c>
+      <c r="D110" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="E110" s="8"/>
+      <c r="F110" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G110" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="H110" s="9">
+        <v>1</v>
+      </c>
+      <c r="I110" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J110" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="K110" s="8"/>
+      <c r="L110" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="M110" s="8"/>
+      <c r="N110" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A110,"', '",B110,"', '",C110,"', '",D110,"', '",E110,"', '",F110,"', '",G110,"', '",H110,"', '",I110,"', '",J110,"', '",L110,"');")</f>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="111" ht="38.7" customHeight="1">
+      <c r="A111" t="s" s="3">
+        <v>242</v>
+      </c>
+      <c r="B111" s="9">
+        <v>2</v>
+      </c>
+      <c r="C111" t="s" s="3">
+        <v>246</v>
+      </c>
+      <c r="D111" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="E111" s="8"/>
+      <c r="F111" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G111" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="H111" s="9">
+        <v>1</v>
+      </c>
+      <c r="I111" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J111" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="K111" s="8"/>
+      <c r="L111" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="M111" s="8"/>
+      <c r="N111" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A111,"', '",B111,"', '",C111,"', '",D111,"', '",E111,"', '",F111,"', '",G111,"', '",H111,"', '",I111,"', '",J111,"', '",L111,"');")</f>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="112" ht="38.7" customHeight="1">
+      <c r="A112" t="s" s="3">
+        <v>242</v>
+      </c>
+      <c r="B112" s="9">
+        <v>3</v>
+      </c>
+      <c r="C112" t="s" s="3">
+        <v>248</v>
+      </c>
+      <c r="D112" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="E112" s="8"/>
+      <c r="F112" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G112" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="H112" s="9">
+        <v>1</v>
+      </c>
+      <c r="I112" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J112" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="K112" s="8"/>
+      <c r="L112" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="M112" s="8"/>
+      <c r="N112" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A112,"', '",B112,"', '",C112,"', '",D112,"', '",E112,"', '",F112,"', '",G112,"', '",H112,"', '",I112,"', '",J112,"', '",L112,"');")</f>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="113" ht="38.7" customHeight="1">
+      <c r="A113" t="s" s="3">
+        <v>250</v>
+      </c>
+      <c r="B113" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C113" t="s" s="3">
+        <v>53</v>
+      </c>
+      <c r="D113" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="E113" s="8"/>
+      <c r="F113" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G113" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="H113" s="9">
+        <v>1</v>
+      </c>
+      <c r="I113" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J113" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="K113" s="8"/>
+      <c r="L113" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="M113" s="8"/>
+      <c r="N113" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A113,"', '",B113,"', '",C113,"', '",D113,"', '",E113,"', '",F113,"', '",G113,"', '",H113,"', '",I113,"', '",J113,"', '",L113,"');")</f>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="114" ht="38.7" customHeight="1">
+      <c r="A114" t="s" s="3">
+        <v>250</v>
+      </c>
+      <c r="B114" s="8"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
+      <c r="F114" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G114" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="H114" s="9">
+        <v>1</v>
+      </c>
+      <c r="I114" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J114" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="K114" s="8"/>
+      <c r="L114" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="M114" s="8"/>
+      <c r="N114" t="s" s="3">
+        <f>CONCATENATE("INSERT INTO APP_REF_DATA (DATA_TYPE, DATA_KEY, DATA_VALUE, GROUP_NAME, SUB_GROUP_NAME, APP_NAME, MODULE_NAME, STATUS_ID, STATUS_TITLE, CREATED_BY, UPDATED_BY) ","VALUES (","'",A114,"', '",B114,"', '",C114,"', '",D114,"', '",E114,"', '",F114,"', '",G114,"', '",H114,"', '",I114,"', '",J114,"', '",L114,"');")</f>
+        <v>252</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9038,16 +9383,16 @@
   <sheetData>
     <row r="1" ht="38.25" customHeight="1">
       <c r="A1" t="s" s="28">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="B1" t="s" s="28">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="C1" t="s" s="28">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="D1" t="s" s="28">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="E1" t="s" s="28">
         <v>3</v>
@@ -9080,7 +9425,7 @@
     <row r="2" ht="14.7" customHeight="1">
       <c r="A2" s="29"/>
       <c r="B2" t="s" s="28">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
@@ -9237,10 +9582,10 @@
   <sheetData>
     <row r="1" ht="14.7" customHeight="1">
       <c r="A1" t="s" s="28">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="B1" t="s" s="28">
-        <v>243</v>
+        <v>259</v>
       </c>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
@@ -9248,13 +9593,13 @@
     </row>
     <row r="2" ht="63.75" customHeight="1">
       <c r="A2" t="s" s="28">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s" s="28">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s" s="28">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="D2" s="31">
         <v>5000</v>

</xml_diff>